<commit_message>
added line c icon
</commit_message>
<xml_diff>
--- a/Icons/subway.xlsx
+++ b/Icons/subway.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick.Grant\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick.Grant\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CC3C6B-8C89-4C32-A4B9-D114B183E78D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FDA1AC-3003-4039-9BF4-BC75F717074C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-300" windowWidth="25440" windowHeight="15540" xr2:uid="{3BE42E33-BF49-4EFB-BBBF-EA02E3F1D165}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{3BE42E33-BF49-4EFB-BBBF-EA02E3F1D165}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F39A3D-0F7C-4327-8CC5-D5A6F92E0241}">
   <dimension ref="A1:AO42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AR30" sqref="AR30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="AR32" sqref="AR32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3897,13 +3897,13 @@
       <c r="AG33" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AH33" s="3" t="s">
+      <c r="AH33" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AI33" s="3" t="s">
+      <c r="AI33" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AJ33" s="3" t="s">
+      <c r="AJ33" s="6" t="s">
         <v>31</v>
       </c>
       <c r="AK33" s="3" t="s">
@@ -4011,7 +4011,7 @@
       <c r="AF34" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AG34" s="3" t="s">
+      <c r="AG34" s="6" t="s">
         <v>44</v>
       </c>
       <c r="AH34" s="3" t="s">
@@ -4023,7 +4023,7 @@
       <c r="AJ34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AK34" s="3" t="s">
+      <c r="AK34" s="6" t="s">
         <v>48</v>
       </c>
       <c r="AL34" s="2" t="s">
@@ -4130,7 +4130,7 @@
       <c r="AF35" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AG35" s="3" t="s">
+      <c r="AG35" s="6" t="s">
         <v>56</v>
       </c>
       <c r="AH35" s="3" t="s">
@@ -4249,7 +4249,7 @@
       <c r="AF36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AG36" s="3" t="s">
+      <c r="AG36" s="6" t="s">
         <v>68</v>
       </c>
       <c r="AH36" s="3" t="s">
@@ -4368,7 +4368,7 @@
       <c r="AF37" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AG37" s="3" t="s">
+      <c r="AG37" s="6" t="s">
         <v>80</v>
       </c>
       <c r="AH37" s="3" t="s">
@@ -4487,7 +4487,7 @@
       <c r="AF38" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AG38" s="3" t="s">
+      <c r="AG38" s="6" t="s">
         <v>92</v>
       </c>
       <c r="AH38" s="3" t="s">
@@ -4499,7 +4499,7 @@
       <c r="AJ38" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AK38" s="3" t="s">
+      <c r="AK38" s="6" t="s">
         <v>96</v>
       </c>
       <c r="AL38" s="2" t="s">
@@ -4599,13 +4599,13 @@
       <c r="AG39" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AH39" s="3" t="s">
+      <c r="AH39" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AI39" s="3" t="s">
+      <c r="AI39" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AJ39" s="3" t="s">
+      <c r="AJ39" s="6" t="s">
         <v>107</v>
       </c>
       <c r="AK39" s="3" t="s">

</xml_diff>